<commit_message>
added save codebook + df backup functionality
</commit_message>
<xml_diff>
--- a/src/uploads/annotated_transcripts.xlsx
+++ b/src/uploads/annotated_transcripts.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>autofill_Sentiment</t>
+          <t>Language</t>
         </is>
       </c>
     </row>
@@ -470,11 +470,11 @@
         </is>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>French</t>
         </is>
       </c>
     </row>
@@ -490,11 +490,7 @@
       <c r="C3" t="b">
         <v>0</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -508,11 +504,7 @@
       <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -526,11 +518,7 @@
       <c r="C5" t="b">
         <v>0</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -547,11 +535,7 @@
       <c r="C6" t="b">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -573,11 +557,7 @@
       <c r="C7" t="b">
         <v>0</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -593,11 +573,7 @@
       <c r="C8" t="b">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -613,11 +589,7 @@
       <c r="C9" t="b">
         <v>0</v>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -633,11 +605,7 @@
       <c r="C10" t="b">
         <v>0</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -655,11 +623,7 @@
       <c r="C11" t="b">
         <v>0</v>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -675,11 +639,7 @@
       <c r="C12" t="b">
         <v>0</v>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -693,11 +653,7 @@
       <c r="C13" t="b">
         <v>0</v>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -711,11 +667,7 @@
       <c r="C14" t="b">
         <v>0</v>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -741,11 +693,7 @@
       <c r="C15" t="b">
         <v>0</v>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -759,11 +707,7 @@
       <c r="C16" t="b">
         <v>0</v>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -779,11 +723,7 @@
       <c r="C17" t="b">
         <v>0</v>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -805,11 +745,7 @@
       <c r="C18" t="b">
         <v>0</v>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Neutral</t>
-        </is>
-      </c>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -825,11 +761,7 @@
       <c r="C19" t="b">
         <v>0</v>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -843,11 +775,7 @@
       <c r="C20" t="b">
         <v>0</v>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
+      <c r="D20" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>